<commit_message>
[IMP] add c++ pipeline template
</commit_message>
<xml_diff>
--- a/src/main/resources/script/db/init-data/devops_service/devops_service/devops_pipeline_template.xlsx
+++ b/src/main/resources/script/db/init-data/devops_service/devops_service/devops_pipeline_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12690" tabRatio="815" firstSheet="1" activeTab="6"/>
+    <workbookView windowWidth="28800" windowHeight="12690" tabRatio="815" firstSheet="1" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="362">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="372">
   <si>
     <r>
       <rPr>
@@ -1976,6 +1976,12 @@
     <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAfQAAAH0BAMAAAA5+MK5AAAABGdBTUEAALGPC/xhBQAAAAFzUkdCAK7OHOkAAAAkUExURUdwTPz8/G4+nv///1wokvPw9FkpitrN5aWNvo9xr8Cs0H1aojtjLeEAAAACdFJOUwBFcCV4JwAAGaxJREFUeNrsnUlvGzkWgPu3cMpL7KNAyK2jQTCd9pEwbNk3gah4uUmTpa2b7HSWvsmwZ3pykyedTPomxHaWPzdVqiqpFtbG4iaDrxsIkMSIP3/vkY9LlX76yYYNGzZs2LBhw4YNGzZs2LBhw4YNGzZs2LBhw4YNGzZs2LBhw4YNGzZs2LBhw4YNGzZs2LBhY7mjJSt2d198fvP2/RQ4CCGw+e3PNx9f7O5K++fMQIctuHf26f10laIoKHJdiunmt3cfn5Hor8GHgw5bMyr44tN74JG6XqBYYJ/epcDDJw/OukcE9z5NHQ8bFYS7/eid7x4+pISHZ2/vqK83BkqT3J53D97t/Vuwes0J//L9KqWoPGbw299ekweCDs/Ghbpj4sNf6COB5rWhk9bZH94ghuqF63792CJkudH33vozWV107yt6X5+1WmRJ0b3pGb68Q66LOMKbAXdeExEzvB7rB+9d5HI5d/1R0X30YVmtv/zCJTzW6O0IGOuVo8NW+2+Xoobh0u/PmjY4qtFh62DsouaBmye9YnTSennX3HmQ9tuvYaORXim6N7L/tsoxuOWZ/w9pwq7WevuP2YwmBh4j9+tgWay3R268L23GPSv49cFSoJOIXGDgowF3zitDh63OtXByz/uTD6Zbh609CeQz9memW/fIZaAjFx8P+Dp6VegH15QiJIf9yY3B1kn7mmIkKzzvpqJ7bfsFkhneOA/NRCdwJCvbo7FunWMFr8T631LBZ/X+vX5PKx8dwt/kjO1J+H8R89BbL70Vi2ztFLmvzUv4g1WkJHofDEMnnS9UDbp7elOv3GWjwwtF5P4UR8yxDiEcInWBv9fSLtn6vqsQHblX0Bj0gy+YqmQ/vTEEHcILldy4ZrlLRCetoVLls7hvVW7rpKFDdTN6cnaH+q1DeK1eureAJbDisYxE6/6iRTk89WY47dZn85oG7+4r3ejt35GmeFJxDScLnQxdXej4Xqt10lmlutDpdrV1jCR0+DtG2tBRtcZGDjrsIm3SvYzHV1W0y0Fv3yH5OzNFvfxAl3XYdynSl/Hej31DF/qBi/QGdSuMdDLQ4YVu9EpLOPHoBHYp0h64fNdCPLq3bMHawf2eDqpP+K72dPdnVnyr3Dps32FkQMLTnQFRiw51bM3ktfJEJTpptVeRIei9gVrrxBTpiOI1qNR6e+oYIt1FveILB6KtDwEwRTty1xRah+0pAI4p6CXahaJDX7pB6HitaJAXa92XbhC72xsoQofQl+6FKdIpWivYohRqPZBujHYPvWjPQiQ66QKj0P2Uv1WU8GNgGDtGO0oSfi4dmDO304IdSoHocLRANyflj4kC9AMQC2MyHr3Ku0IqEH0SR3eMQT+RX+ttAAzU7sHfSEcfJtHNqfZ7yehwMbOZhn5KJFvvAmAou3vFHuhEoZNJGt2caj+Sa72TITdHO74hMtGHWXRztG9ItA7hFJirHZ8yOzpB1veBwejeQCfR+gQYzX4kD70N2GHOQCcN/TAH3Zhqv5WFHl+uAiMXMcdEDjrsAGC6dsbULsT6MBfdlO0avCbFemblYmLKM6Z2Eej5+W5QtZ/LQCd9YD472pCS8OMidGBMxotHJ/uF5Mak/KUE6/1idEMGefwUCkffHYNl0O6e7gpH3wJLgU4zY3xz9CFYDna8kTqCaowOx6XowMwxvjF6p5zcDO0Y3Yi1ToYV0A0Z5NcEWx+BpdF+JNQ6aU+XBx0NhFrvArA87MnHA5pan1RDN2KQxycircPpEqGj5KK9IfoWAMuk/Vyg9WFldBOqPblN1RB9tFToyaOIZuhtAJaKnQ5EocOtGugGVDvGl0SU9T5YLu3ur8Ksj+ugm9DJHwuyDtu1yI3QPhBkvVsP3YRqvxKE3gfLpj2+Odko4cfN0VXX/7EQ63VLncnOgU6b/LzcGyHWu7XRGYM8pmy8gu8++Dq+56XxJRSB3gcCtCd4KloPNh5qfkEYT4VYv6iPnhnkKZ59dl/mJbtuQUQC3WqRRF/sUjVAL9mb+v45jGmh9qPgL90l0/JzQXwKUDY+V4pPydqJPd/Mj17WwF8y6yKDHiZg8mVduOjJ83YAc1XxNWCph8rd+SFMA+uHxVV9yf4RpdhpiH6d/O0i9A5NNyeF6E5Su7vS3HrZttxlzvRfxToqt86LTo8EJHxJQxPNIjD5UExKO2Wi03LrLh86XjwZwI1e1tA4lzkbeA7T+rUq64ubk/zWSy5TgEXvkJoKHCHWudHpZWP0fmXrqYxPVvtj6dbTc8rjxuijytbTCeIwvhF51jM98RFsWuvT6tYLMp6WWCc5MDgzr+d8uFvbzR5ENEQvPVe/jH0rk3ztxdbJjCn5356P7obWSfBBzST6IUH/U1zh4g8Y1t3wnJ0b/edy9Nj7FvM7+SLr0CeCKbcwmtyIHxD6sP4v87l0/jv+LyRb69E1Mm70snMXJ1brmXbfySQ803r7DSveBgDrqd9+F6TIPvNvs85guNEndazD/Ix/HKhidnOdopVbeuEWdGnkec46LxYnsBF66eZUwnpmV8MpHuZC6506HwwVNqjPy7/ktFmtl29OXcZH6IPcdfvjgh6+U2cnKkKvsFMTvLKFE738yCm03iHsLsCpMsLXQ4eV0c8bWT+saL0T/DPkMEd74bwuyTq6bYAOy/flIuu3OY8LOJWsS6l19Gsj66OK1tsnOQ9FORXmdUnW6XET9PI7NIF12H5EcvoAp3xel1TrdKfJMFfh9CG0DoL3+DIekNFnHQ/40Un5nYKw1uH0FuY0AlWsYynDXDDEc1o/rGodTtdhXuery3r4nCcner+q9d0pGAS97Bb7KEZ9rWOEHzdAn1S3DnIz3int4SVZR780mNfHFawHw9sURBnfZ2oX3sNXujbpf2986FXuQ8+tg/Ath1usEzisoYdHaHvAbb3C3DYf4YETbiXtTlnaNczr4Sk7H3qV+3IL6xutvCW+o2eED2Y3PvRuHesADHLvEjta5nVvAQN50fu1rIOrxft1M9cstFif5Rof+qSe9fyMB054pUltrc9eQseHPq5nfXOQf/nmqRbrx7zoVZ59iFsHr2Buxq9pqfUe57xe7dZYzHpRxq9pse7fDueyXumJxnk3N894CBkZf6+l1t1zTus/17UOzoPP0WznWFfdw89OYLisd0HNWo/SmrGvtaajh58tW7nQh7WtR+8vzv7QVnT08LPDJy70fm3r4Hx2HAj3ao7wsmrdf9qPC31S2/o848eGjPBHnMPcqL71aGM2s7N1r2Vep08IH/q0vnUv49lHEXqs4x0+9EodTcp6NH9n9nfu9dQ6HvCh9zisBxk//7iI+U9Ij3X/9hwP+hao2835Ed5g6RhR6/5mBQ96pWYubT1iTL/BR5f1Sy70Q55a7z1iv6dMT60j+g8u9CGX9Sjj95k9/AX7Lk36cQjkUjHW0RoXep/HeuSXpMb4MOFHDusG1dnZ2YuPif/PXlxQIehPudAnfNbXg9VbKuNXonVN1Tuy/xRj/YQLfcRnHdywbsxG1pPXR/PRyXMhte79pHjQx3zWo8O35DZVWOuj5IXpAuv/FWP9mAe92vOcmXndy3jWUxH384W8k7UO/Xuiqf+fi0E/JTzoU07rp+HhW5eZ8ImML7D+lxj0Hg96xXcvZWsd3DJuzC7Q4zdnC9AF1XpvwIMOOK17GU8yG7PBCE9GyQvT8q27POgdwGt9J/wsxS7beuzmLI/1euj4Rho6y/r88K0MvcA6+Usj+ha3dXASZvyINcLH2BXUOj7nQN/ntx4evsU/+W0xr8e1y+/m8BUHepffOiPj1xIb9E5y5fbjz2/p+PFFDDq6lYbOtB4cvsF4xq8kzyZSKzdGUI3oh4Czm4sdNx/mWI9uzuau17Gg9TrCKxzo/QbWwav0o2KJWp9rl75L461apaGzaz3IeBLbyr9PHcY53Ls0xqDnWN8M33E4zEn48CUmhqJPmlgPL1iQTi66o2RvDqETaeg51p3gKGLx0RnxHn6R8Qqs86CPGlnfTD0VkbHus6uo9V+koedYB+A8OcZn0YES65gHfdxgXvdZYeIo4j6L7vCdvtSs9SfS0HOtR8fNffa8HmS8goQ/lmgd5jwadZ64MctIeOCoqPUd9dajFA//ZIWFjhWgn3KgTxtajzJ+kmsdOApqfVsaer715FEEo9a9UGCdBx00tB5dsAg2Zu+ZF+qWGr3A+nr4/olJbsI/WOtRxndz0Tfl1zpGOqyvxo8iMj28KutIovWcbi44bvYP2mcv79CW8Fqsz58D6j5M9KJanx++5Y3wCmpdl/X1xVGErnmda5ibNrceZjw81JfweFuP9fAows/4pZrXRVhfn7+8Q9e8jno6evjEUcSGrh6+p36XJvjTq+h1NRtQU8LrWK8HRxHRHfENXbV+qmGXJpHxw/WiWkdIXq0f67IejfGd4HUOOT08kGidB30kwjoIPz9z91tRwiculAlGP1K/D586ivgfKUIHZqFPhFh3wuPmA1JQ66CGdn1nbps/6lmPnm6GRfM6qKFdxZnb/9s7l57GlSyOz0eYz2CZToKXpVK4LKOWb8/0rktWIL1DEReaHVEUSO9gMjTNLq0MBHbNzQ0ddpEYAny5cTl+JmXHroddGdW57ygX8sv/1DmnTpWriIvMs079YZpFdX+5Odnh08te1Pr6Jv6sJ5lU184TLoYLoe83zUUrDP0TQcH7peP0kqu50OJbUl7XtVrNNNPtJMram/udzzaiTXxgM4xueV6pegWFzgQmql4dYrtbtBedx6R1gw/6YPkI7ZVjPerxRHQ3DqBF+4sHOqd9cy0CwErV7flqcCA0GT3L5ug89s3tEFzX/aifMqke8njyWM+GDsVvFN2Kazw4DacMqmv+reAwf9Wptgcvbwr3TpQLx7kUqnvd2EIcntN++DKAy0dRpFD9H4gGHRaHvvwASIVwAZCeAl27hxzH+jwfpEbn8+yL/0mPI6qjlejPxTl8kwadQOPGq3DDIZXqZUSDnpzXUzZxqR72Ijzi515JEXmK68d8V2Ry//beK13So8NEh0dCH/EjPNi5uRzlUqnuLb7xGOsfcniwk/Q473lk3+vcE5y6fgV6GeGnNe1SdUn15Sc6vcc8lw6s8tBhFtWpHucl3WZWtktZeBoN+87cY7iimTN0bUp+OWRvtt3Zf768kacve8MX/I7/pgzwB5DXo/uzcefXO02gvcNXeTTfm819+y8SzP6+ia8FSdm6N/8QeGADb8vQnE1jJXHHdPBHN3mSmxsCD2fh7/JNk989xpSHs2wVg871Im/KI3mqNW3tRzvlQUxVbf1lpzx+K+WJDVLLfoTEHbUnOfohHTr4U1t79gORZ0vKPdq/iDxMVWrZm7SHqX7W1l522iN0t7R1l5324GS4vf7o5yIPSZebnfaQdGuqrflo37NEXoggtezUFyIUmNg191gD9rQu8PITqWX/Q+SVN1KjOxe60aFvaevNznDRUbVQdPYgb9Jfb1Wdrjf6Hv2lZoVmNw7sh4D6eqt0R8muaLAaL3hn2DT30W66+24o0Tlkt9uxha3z0M9ZdtO9RI4SnTm7HV1Y0EG3YOcq7yDPclkpZM1uRs8KbCd3dJYralmz24XFhs7IznAxMWs/+hWxojNV8jWW66jBv1jIK21M3L18M95uxpToOuO8jR6dae7mDPRfc8epzUY7eef2L0zoLCG+jMlPdd8HHvKu5J9Y0BFLiB/Qjm9e6OdMY50hxBs2eZ1DJUzNPr95nhod0n/2ko3OZRGDNsi7l8vRojPEOTvI8Zn50cr+BbKhU+tWsUXn1OVh6E6xoFNvqNm00WMnfjX/b1rCW2pMsps/GNGpV2Ce7CAX5+/GzWQ8ebgLg9YwpzH0XtONm2/fLqcM6KZ5z4hOXcqO4v29bJd2EKF6sO1yczJ51LRZ26q7jjLrWBBY3T49e/MIMaLTxjmc2o6T6lun3glcBO46r7u7U8vzt6DGlD7IH0CA2NApuxUfYof60SiY0Xjv2MAu4tS9Drrhfzm71LKb3g2a9Ohb1FEuZqhfu1S4hbE9DdArlo8+WPxydPooxzDWKeu5Z8tqxLt7vTuZ4H+ixwD92UIuuvMl1LuddlAJZ2bfN70HbuhVp6znenFR7hlj4V7VC3b8hp8OdkdW43J48dMr/u+csOe7DnWUY0CnjHM2Onk/Cpbyat6qxf/a91TfcQp+Yzof6Y0pTnavftzLLvsBYEaHn2lz29e48OcF9lc/C9jodef9ujvZ/en/lM+UJd0GOzplnGtb6GdckPOGkDHyxvIGHt3TYLK7vRwxMspunrM7PKKbg7R95ZYGws6eR4MrPm+sB1P7kMOUg8GeEb3W4qA6+DdNRRODjl8/jtT5fU/1r6Fi6Cz09jMq2Q8gD/RjjqqXI5UOpvzTQz8jVQS90I/J5O+/Ax7ov9Gpjs5WVzoj1wc2QkO9FG5rDUJOkkH2pl/QsKFXOapeilY6A9fP/UHv5vilN2Sr5JvvvWkbIzrq8xvrT9FKx/tPW/VGjUT7HC4PMsh+CBAPdKrBHpPc7LH7KVra7XglTegtp/hZv8sb26KVUeYODbPqu9wcXu9Fp7KlAH03NP7tIi5YsvpM0aUzB5ALOtVgvydXcwvom9DaWhwHIytqNOjNFh/VqfaVxDRpelFnsNHJqpPR07Kbh4gXOsVg75FXXmJUT0Lfzd6cbf4TcEKH2ZeP9OtQusqsemMSssfsPfn9H7zQaTaRlYirTkthDs6RF8b6sREYzXLEfouXw0OKMj4080xw+FKQ13cXKzyGpZgPiJvqFGswBnnF7SkatryKJYzeS16qa2boSPJA36YK8Q1ie2onWsgeL6IP4vo7qWU3zzmiUyxEDEI9icj0pUGIeuGx/rxiVT7NEitHh0fZG3SbRI+3Q0C1H6n5+ouql+J6uSllN70lVk6qZ69lKxYJITqtqXgZMIxeJrpLBvRwFcuOTpPe8GLKY3KVVwr15nbDjfqfDLI337cQT3SKp5rxrorGNHEB1g/mkbnsKDLYp1mDvHkQPeiHdazTpDe8enganORi/PLc+TE0JvpLqjs9St/jn8+yyh5Nbeyq06Q3Z3HNP3TW2zfXDsq8nh8NIujloD1beyWuWa5+9IEnOsX603wx+cQ5afnte9sNlXjhqTvVdd35ar4S0J1VmdPpXq1m3LaJ6Emym0eIq8NTeby7plq3pyDjYOWwgpsQjcvhEG8d9oZ9ZKzr1/P9pcNv45iVaj35/CHOqtMswhjz+SeKzj6v5yvMCIZGfUR1110ggvZbiH3dRPZzxBudZsU12D8R2kPxcbS8VzqKrj0H7anGNFslv3+EuKsOaZqTsxB7d7r4YjCrXUA3/H30cdst9Xh/h9zR6bbLVsYew6Wf5vTZXPdugFXqdCJHuXnsJ/2Mlbz5/gfg7vDAottjMJuMO93JZcRvjdtJZ+Gl5f9tMnm4yl7SfVw6uJADOpXHex9U42164h54zg4PGppMppP9vSdCdZZd0nmhvz9CQAR6gefUpGVfrN+5oW9Lha6R63chDl/ceVypZT9EghwefZZbdtN8AoIcHlY1yWW/F4VO053MEd0MtgnyRwc7csveE4aOYGFnLqYa7R8REqe6ZKk9KjspqfNDh5Kldi2a1JE4dATgT3llPwAiVS/4gKIkdNMcCEaXaw4TZj9CYtGhbIFO85N6CQhWHUlW0Xmym3v3glUv+hC6eI//AoBw9IaMspvkSo4zumRTVwe9GdkkKAxdtvyG2WMzG190JFt+0xIyG2fVoYSyP8Fc0FHBJ/ARZD9q5aO6dPM37V0p4cNyRYeyyW60YE7o0sleAigvdMlGe6LovFVHMsmuPyfeCscZHcgke7LovNGlmrsmi85ddYlkXyE6d3SJZF8hOn/VQVWSSr6yQnT+6FCWCdwA5K46lGMChy9GRzmj0zz9JsB6AOauOpBiOaKMACgAXYYu3T0oBF2CBPcMikG3ZzEFR7rDFoAWWmFC0AvvUA4A/PvfBFgKclhspNtExaEDsF1gKW/YMa5AdHRabIwrEr24tZiyc1d7cegAFZbcR6BQ1VFhLUq3K1Wk6naUPyvG3YtHt+vZAqL8xxGQAR0UEOWvgRzo+Rc2m0gSdFD/T95NKSAHOoQ5bxuu9YL2RNGqw3yH+3XoNxeNDoB1lV9Gf0UyocMce9OVVmjvtwSqw9yyu5fRpUG37SQf8gsgH3o+oe564ZfKgQ4fxZO/LjSfJVEdQOFhfrbYdpcEHYGq4EncrAWhnKoDwezl1nIhKQ06qPdFJvRlR9uWBR0BKE73ShvC5dagPKqL073SJvyyllTooHqXk7dLpzpA1SsREQ6S1tHbcqGLYJ+1Y0aXJRe6nXN+ia3hgl/Ulg0dwROe87gLFLdhBjZkQ8fzOG7sxkWCe1kSooMGp0D/MkrsDsmIDqpcBvxtK3GLFJQQHa+CMjv9O+MCJW8Og1KqjnPPFdu5W7PRym9YSnSI/zjps8Q3BFZtCJRWdSz8L+dmtuwtZ+O2neb7lRgdgO4lDfpNJ51ryYxux6lu5jz3MkYr976uger4A3avphlc/WaM3B0bq012dBu+85AS3vjeSam49KrD+VosgPWTu5X0xsv3th/W4f+Dw3ufs/4wfIs7YlPX3oZY8Iw/ck3QHfruw+XbdG+hatPebr6P24ji560PujPlsDrdh2/Du7e5iw+/fR93LIvyqxSCrkyZMmXKlClTpkyZMmXKlClTpkyZMmXKlClTpkyZMmXKlClTpkyZMmXKlClTpkyZMmXKlClTJpP9D2/I6A663xVoAAAAAElFTkSuQmCC</t>
   </si>
   <si>
+    <t>devops_ci_template_category-8</t>
+  </si>
+  <si>
+    <t>C/C++</t>
+  </si>
+  <si>
     <t>流水线模板</t>
   </si>
   <si>
@@ -2080,6 +2086,12 @@
     <t>.NET Core: .NET Core构建镜像+容器部署</t>
   </si>
   <si>
+    <t>devops_ci_template_pipeline-10</t>
+  </si>
+  <si>
+    <t>C/C++:构建镜像+容器部署</t>
+  </si>
+  <si>
     <t>流水线ci变量</t>
   </si>
   <si>
@@ -2162,6 +2174,9 @@
   </si>
   <si>
     <t>devops_ci_template_stage-17</t>
+  </si>
+  <si>
+    <t>devops_ci_template_stage-18</t>
   </si>
   <si>
     <t>流水线模板任务分组</t>
@@ -2401,6 +2416,12 @@
     <t>registry.cn-shanghai.aliyuncs.com/c7n/cibase:0.11.4</t>
   </si>
   <si>
+    <t>devops_ci_template_job-29</t>
+  </si>
+  <si>
+    <t>C/C++镜像构建</t>
+  </si>
+  <si>
     <t>阶段任务关系表</t>
   </si>
   <si>
@@ -2480,6 +2501,9 @@
   </si>
   <si>
     <t>devops_ci_template_stage_job_rel-23</t>
+  </si>
+  <si>
+    <t>devops_ci_template_stage_job_rel-24</t>
   </si>
   <si>
     <t>devops_ci_template_step_category</t>
@@ -2816,6 +2840,12 @@
   </si>
   <si>
     <t>devops_ci_template_job_step_rel-45</t>
+  </si>
+  <si>
+    <t>devops_ci_template_job_step_rel-46</t>
+  </si>
+  <si>
+    <t>devops_ci_template_job_step_rel-47</t>
   </si>
   <si>
     <t>步骤执行参数</t>
@@ -3019,29 +3049,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFFFFFF"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3055,7 +3065,98 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3070,62 +3171,6 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="等线"/>
@@ -3135,22 +3180,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3239,7 +3269,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3251,19 +3329,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3275,19 +3347,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3299,61 +3413,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3371,7 +3437,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3383,43 +3449,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3526,17 +3556,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3557,16 +3596,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3589,16 +3628,16 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="double">
+      <right style="thin">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="double">
+      <top style="thin">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
+      <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -3614,25 +3653,16 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="42" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -3641,138 +3671,138 @@
     <xf numFmtId="41" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="14" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="20" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="31" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="31" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3786,6 +3816,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4246,8 +4279,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.25" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="15.5851851851852" style="11" customWidth="1"/>
-    <col min="2" max="2" width="10.3333333333333" style="12" customWidth="1"/>
+    <col min="1" max="1" width="15.5851851851852" style="12" customWidth="1"/>
+    <col min="2" max="2" width="10.3333333333333" style="13" customWidth="1"/>
     <col min="3" max="3" width="28.0814814814815" customWidth="1"/>
     <col min="4" max="4" width="35.3333333333333" style="6" customWidth="1"/>
     <col min="5" max="5" width="38.5851851851852" customWidth="1"/>
@@ -4263,79 +4296,79 @@
   </cols>
   <sheetData>
     <row r="1" ht="64.5" customHeight="1" spans="1:8">
-      <c r="A1" s="13"/>
-      <c r="C1" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
+      <c r="A1" s="14"/>
+      <c r="C1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
     </row>
     <row r="2" ht="18" spans="5:5">
-      <c r="E2" s="16"/>
+      <c r="E2" s="17"/>
     </row>
     <row r="3" ht="49.5" customHeight="1" spans="3:7">
-      <c r="C3" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="17"/>
-      <c r="E3" s="18" t="s">
+      <c r="C3" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="18"/>
+      <c r="E3" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
     </row>
     <row r="4" ht="18" spans="3:7">
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="19"/>
-      <c r="E4" s="20" t="s">
+      <c r="D4" s="20"/>
+      <c r="E4" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="F4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="22" t="s">
+      <c r="G4" s="23" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="13"/>
+      <c r="A5" s="14"/>
       <c r="C5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" ht="18" spans="3:5">
-      <c r="C7" s="23" t="s">
+      <c r="C7" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="24" t="s">
+      <c r="D7" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="25" t="s">
+      <c r="E7" s="26" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="3:5">
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="27" t="s">
+      <c r="D8" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="28"/>
+      <c r="E8" s="29"/>
     </row>
     <row r="9" ht="51.75" spans="3:6">
-      <c r="C9" s="29" t="s">
+      <c r="C9" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="30" t="s">
+      <c r="D9" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="31" t="s">
+      <c r="E9" s="32" t="s">
         <v>15</v>
       </c>
       <c r="F9" t="s">
@@ -4343,56 +4376,56 @@
       </c>
     </row>
     <row r="10" ht="51.75" spans="3:5">
-      <c r="C10" s="32" t="s">
+      <c r="C10" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="30" t="s">
+      <c r="D10" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="31" t="s">
+      <c r="E10" s="32" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="11" ht="69" spans="3:5">
-      <c r="C11" s="26" t="s">
+      <c r="C11" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="30" t="s">
+      <c r="D11" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="31" t="s">
+      <c r="E11" s="32" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="12" spans="3:5">
-      <c r="C12" s="26" t="s">
+      <c r="C12" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="30" t="s">
+      <c r="D12" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="E12" s="33" t="s">
+      <c r="E12" s="34" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="13" spans="3:5">
-      <c r="C13" s="26"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="28"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="29"/>
     </row>
     <row r="14" spans="3:5">
-      <c r="C14" s="26"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="28"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="29"/>
     </row>
     <row r="15" ht="34.5" spans="3:5">
-      <c r="C15" s="34" t="s">
+      <c r="C15" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="35" t="s">
+      <c r="D15" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="36" t="s">
+      <c r="E15" s="37" t="s">
         <v>28</v>
       </c>
     </row>
@@ -4402,30 +4435,30 @@
       </c>
     </row>
     <row r="19" spans="3:5">
-      <c r="C19" s="37" t="s">
+      <c r="C19" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="D19" s="37"/>
-      <c r="E19" s="37"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="38"/>
     </row>
     <row r="20" ht="18" spans="3:4">
-      <c r="C20" s="38" t="s">
+      <c r="C20" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="D20" s="16" t="s">
+      <c r="D20" s="17" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="21" ht="18" spans="3:4">
-      <c r="C21" s="38" t="s">
+      <c r="C21" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="D21" s="16" t="s">
+      <c r="D21" s="17" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="22" ht="18" spans="3:4">
-      <c r="C22" s="38" t="s">
+      <c r="C22" s="39" t="s">
         <v>35</v>
       </c>
       <c r="D22" s="6" t="s">
@@ -4433,7 +4466,7 @@
       </c>
     </row>
     <row r="23" ht="18" spans="3:4">
-      <c r="C23" s="38" t="s">
+      <c r="C23" s="39" t="s">
         <v>37</v>
       </c>
       <c r="D23" s="6" t="s">
@@ -4441,25 +4474,25 @@
       </c>
     </row>
     <row r="25" ht="69" customHeight="1" spans="3:5">
-      <c r="C25" s="39" t="s">
+      <c r="C25" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="D25" s="17" t="s">
+      <c r="D25" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="E25" s="17"/>
+      <c r="E25" s="18"/>
     </row>
     <row r="26" ht="14.25" customHeight="1" spans="3:5">
-      <c r="C26" s="27" t="s">
+      <c r="C26" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="D26" s="17" t="s">
+      <c r="D26" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="E26" s="17"/>
+      <c r="E26" s="18"/>
     </row>
     <row r="27" ht="51.75" spans="3:3">
-      <c r="C27" s="40" t="s">
+      <c r="C27" s="41" t="s">
         <v>43</v>
       </c>
     </row>
@@ -4542,82 +4575,82 @@
         <v>50</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>330</v>
+        <v>340</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>331</v>
+        <v>341</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>53</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>296</v>
+        <v>304</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>332</v>
+        <v>342</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>333</v>
+        <v>343</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>334</v>
+        <v>344</v>
       </c>
       <c r="J7" t="s">
-        <v>335</v>
+        <v>345</v>
       </c>
       <c r="K7" t="s">
-        <v>336</v>
+        <v>346</v>
       </c>
       <c r="L7" t="s">
-        <v>337</v>
+        <v>347</v>
       </c>
       <c r="M7" t="s">
-        <v>338</v>
+        <v>348</v>
       </c>
       <c r="N7" t="s">
-        <v>339</v>
+        <v>349</v>
       </c>
       <c r="O7" t="s">
-        <v>340</v>
+        <v>350</v>
       </c>
     </row>
     <row r="8" customFormat="1" spans="5:9">
       <c r="E8" s="6" t="s">
-        <v>341</v>
+        <v>351</v>
       </c>
       <c r="F8" s="6" t="str">
         <f>流水线步骤模板!E8</f>
         <v>devops_ci_template_step-1</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="H8" s="6">
         <v>1</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>343</v>
+        <v>353</v>
       </c>
     </row>
     <row r="9" customFormat="1" spans="5:10">
       <c r="E9" s="6" t="s">
-        <v>344</v>
+        <v>354</v>
       </c>
       <c r="F9" s="6" t="str">
         <f>流水线步骤模板!E21</f>
         <v>devops_ci_template_step-14</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>345</v>
+        <v>355</v>
       </c>
       <c r="H9" s="6">
         <v>1</v>
       </c>
       <c r="I9" t="s">
-        <v>343</v>
+        <v>353</v>
       </c>
       <c r="J9" t="s">
-        <v>346</v>
+        <v>356</v>
       </c>
     </row>
     <row r="10" customFormat="1" spans="5:8">
@@ -4640,52 +4673,52 @@
     </row>
     <row r="14" spans="4:14">
       <c r="D14" t="s">
-        <v>347</v>
+        <v>357</v>
       </c>
       <c r="E14" t="s">
         <v>53</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>296</v>
+        <v>304</v>
       </c>
       <c r="G14" t="s">
-        <v>348</v>
+        <v>358</v>
       </c>
       <c r="H14" t="s">
-        <v>349</v>
+        <v>359</v>
       </c>
       <c r="I14" t="s">
-        <v>350</v>
+        <v>360</v>
       </c>
       <c r="J14" t="s">
-        <v>351</v>
+        <v>361</v>
       </c>
       <c r="K14" t="s">
-        <v>352</v>
+        <v>362</v>
       </c>
       <c r="L14" t="s">
-        <v>353</v>
+        <v>363</v>
       </c>
       <c r="M14" t="s">
-        <v>354</v>
+        <v>364</v>
       </c>
       <c r="N14" t="s">
-        <v>355</v>
+        <v>365</v>
       </c>
     </row>
     <row r="15" spans="5:11">
       <c r="E15" t="s">
-        <v>356</v>
+        <v>366</v>
       </c>
       <c r="F15" t="str">
         <f>流水线步骤模板!E11</f>
         <v>devops_ci_template_step-4</v>
       </c>
       <c r="G15" t="s">
-        <v>357</v>
+        <v>367</v>
       </c>
       <c r="H15" t="s">
-        <v>358</v>
+        <v>368</v>
       </c>
       <c r="I15">
         <v>0</v>
@@ -4699,17 +4732,17 @@
     </row>
     <row r="16" spans="5:11">
       <c r="E16" t="s">
-        <v>359</v>
+        <v>369</v>
       </c>
       <c r="F16" t="str">
         <f>流水线步骤模板!E16</f>
         <v>devops_ci_template_step-9</v>
       </c>
       <c r="G16" t="s">
-        <v>360</v>
+        <v>370</v>
       </c>
       <c r="H16" t="s">
-        <v>361</v>
+        <v>371</v>
       </c>
       <c r="I16">
         <v>0</v>
@@ -4733,7 +4766,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.25" outlineLevelCol="7"/>
@@ -4907,9 +4940,19 @@
         <v>77</v>
       </c>
     </row>
-    <row r="15" customFormat="1" spans="5:6">
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
+    <row r="15" customFormat="1" spans="5:8">
+      <c r="E15" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F15" s="6">
+        <v>1</v>
+      </c>
+      <c r="G15" t="s">
+        <v>79</v>
+      </c>
+      <c r="H15" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="16" customFormat="1" spans="5:6">
       <c r="E16" s="6"/>
@@ -4946,8 +4989,8 @@
   <sheetPr/>
   <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.25"/>
@@ -5004,34 +5047,34 @@
         <v>50</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>53</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="K7" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="L7" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="M7" t="s">
         <v>56</v>
@@ -5039,19 +5082,19 @@
     </row>
     <row r="8" spans="5:11">
       <c r="E8" s="6" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F8">
         <v>0</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H8" s="6">
         <v>1</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="J8" t="str">
         <f>流水线模板分类!E9</f>
@@ -5063,19 +5106,19 @@
     </row>
     <row r="9" spans="5:11">
       <c r="E9" s="6" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F9">
         <v>0</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="H9" s="6">
         <v>1</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="J9" t="str">
         <f>流水线模板分类!E9</f>
@@ -5087,19 +5130,19 @@
     </row>
     <row r="10" spans="5:11">
       <c r="E10" s="6" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="F10">
         <v>0</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H10" s="6">
         <v>1</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="J10" t="str">
         <f>流水线模板分类!E10</f>
@@ -5111,19 +5154,19 @@
     </row>
     <row r="11" customFormat="1" spans="5:11">
       <c r="E11" s="8" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="F11">
         <v>0</v>
       </c>
       <c r="G11" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H11">
         <v>1</v>
       </c>
       <c r="I11" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="J11" t="str">
         <f>流水线模板分类!E10</f>
@@ -5135,19 +5178,19 @@
     </row>
     <row r="12" customFormat="1" spans="5:11">
       <c r="E12" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F12">
         <v>0</v>
       </c>
       <c r="G12" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H12">
         <v>1</v>
       </c>
       <c r="I12" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="J12" t="str">
         <f>流水线模板分类!E11</f>
@@ -5162,19 +5205,19 @@
       <c r="C13" s="6"/>
       <c r="D13" s="1"/>
       <c r="E13" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="F13">
         <v>0</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H13" s="3">
         <v>1</v>
       </c>
       <c r="I13" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="J13" t="str">
         <f>流水线模板分类!E11</f>
@@ -5186,19 +5229,19 @@
     </row>
     <row r="14" customFormat="1" spans="5:11">
       <c r="E14" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="F14">
         <v>0</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H14" s="6">
         <v>1</v>
       </c>
       <c r="I14" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="J14" t="str">
         <f>流水线模板分类!E12</f>
@@ -5210,19 +5253,19 @@
     </row>
     <row r="15" customFormat="1" spans="5:11">
       <c r="E15" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="F15" s="3">
         <v>0</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H15" s="6">
         <v>1</v>
       </c>
       <c r="I15" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="J15" t="str">
         <f>流水线模板分类!E13</f>
@@ -5234,19 +5277,19 @@
     </row>
     <row r="16" customFormat="1" spans="5:11">
       <c r="E16" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="F16" s="6">
         <v>0</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H16" s="6">
         <v>1</v>
       </c>
       <c r="I16" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="J16" t="str">
         <f>流水线模板分类!E14</f>
@@ -5256,7 +5299,30 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" customFormat="1"/>
+    <row r="17" customFormat="1" spans="5:11">
+      <c r="E17" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="J17" t="str">
+        <f>流水线模板分类!E15</f>
+        <v>devops_ci_template_category-8</v>
+      </c>
+      <c r="K17">
+        <v>1</v>
+      </c>
+    </row>
     <row r="18" customFormat="1"/>
     <row r="19" customFormat="1"/>
     <row r="20" customFormat="1" spans="5:8">
@@ -5352,22 +5418,22 @@
         <v>50</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>53</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" customFormat="1" spans="5:8">
@@ -5432,10 +5498,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView topLeftCell="D4" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.25" outlineLevelCol="7"/>
@@ -5486,30 +5552,30 @@
         <v>50</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>53</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" customFormat="1" spans="5:8">
       <c r="E8" s="6" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="F8" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="G8" s="6" t="str">
         <f>流水线模板!E8</f>
@@ -5521,10 +5587,10 @@
     </row>
     <row r="9" customFormat="1" spans="5:8">
       <c r="E9" s="6" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="G9" s="6" t="str">
         <f>流水线模板!E8</f>
@@ -5536,10 +5602,10 @@
     </row>
     <row r="10" customFormat="1" spans="5:8">
       <c r="E10" s="6" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="G10" s="6" t="str">
         <f>流水线模板!E9</f>
@@ -5551,10 +5617,10 @@
     </row>
     <row r="11" customFormat="1" spans="5:8">
       <c r="E11" s="6" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="G11" s="6" t="str">
         <f>流水线模板!E9</f>
@@ -5566,10 +5632,10 @@
     </row>
     <row r="12" customFormat="1" spans="5:8">
       <c r="E12" s="6" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="G12" s="6" t="str">
         <f>流水线模板!E10</f>
@@ -5581,10 +5647,10 @@
     </row>
     <row r="13" customFormat="1" spans="5:8">
       <c r="E13" s="6" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="G13" s="6" t="str">
         <f>流水线模板!E10</f>
@@ -5596,10 +5662,10 @@
     </row>
     <row r="14" customFormat="1" spans="5:8">
       <c r="E14" s="8" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="G14" t="str">
         <f>流水线模板!E11</f>
@@ -5611,10 +5677,10 @@
     </row>
     <row r="15" customFormat="1" spans="5:8">
       <c r="E15" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="F15" s="6" t="s">
         <v>125</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>121</v>
       </c>
       <c r="G15" t="str">
         <f>流水线模板!E11</f>
@@ -5626,10 +5692,10 @@
     </row>
     <row r="16" spans="5:8">
       <c r="E16" s="6" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="F16" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="G16" t="str">
         <f>流水线模板!E12</f>
@@ -5641,10 +5707,10 @@
     </row>
     <row r="17" spans="5:8">
       <c r="E17" s="6" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="F17" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="G17" t="str">
         <f>流水线模板!E12</f>
@@ -5656,10 +5722,10 @@
     </row>
     <row r="18" spans="5:8">
       <c r="E18" s="6" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="F18" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="G18" t="str">
         <f>流水线模板!E13</f>
@@ -5671,10 +5737,10 @@
     </row>
     <row r="19" spans="5:8">
       <c r="E19" s="6" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="F19" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="G19" t="str">
         <f>流水线模板!E13</f>
@@ -5686,10 +5752,10 @@
     </row>
     <row r="20" spans="5:8">
       <c r="E20" s="6" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="F20" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="G20" t="str">
         <f>流水线模板!E14</f>
@@ -5701,10 +5767,10 @@
     </row>
     <row r="21" spans="5:8">
       <c r="E21" s="6" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="F21" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="G21" t="str">
         <f>流水线模板!E14</f>
@@ -5716,10 +5782,10 @@
     </row>
     <row r="22" spans="5:8">
       <c r="E22" s="6" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="F22" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="G22" t="str">
         <f>流水线模板!E15</f>
@@ -5731,10 +5797,10 @@
     </row>
     <row r="23" spans="5:8">
       <c r="E23" s="6" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="F23" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="G23" t="str">
         <f>流水线模板!E15</f>
@@ -5746,16 +5812,31 @@
     </row>
     <row r="24" spans="5:8">
       <c r="E24" s="6" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="F24" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="G24" t="str">
         <f>流水线模板!E16</f>
         <v>devops_ci_template_pipeline-9</v>
       </c>
       <c r="H24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="5:8">
+      <c r="E25" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="F25" t="s">
+        <v>122</v>
+      </c>
+      <c r="G25" t="str">
+        <f>流水线模板!E17</f>
+        <v>devops_ci_template_pipeline-10</v>
+      </c>
+      <c r="H25">
         <v>0</v>
       </c>
     </row>
@@ -5771,7 +5852,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.25" outlineLevelCol="7"/>
@@ -5822,22 +5903,22 @@
         <v>50</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>53</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G7" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" customFormat="1" spans="1:8">
@@ -5846,13 +5927,13 @@
       <c r="C8" s="6"/>
       <c r="D8" s="1"/>
       <c r="E8" s="2" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>58</v>
       </c>
       <c r="G8" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="H8" s="6">
         <v>1</v>
@@ -5860,13 +5941,13 @@
     </row>
     <row r="9" customFormat="1" spans="5:8">
       <c r="E9" s="6" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="F9" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="G9" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="H9">
         <v>1</v>
@@ -5874,13 +5955,13 @@
     </row>
     <row r="10" customFormat="1" spans="5:8">
       <c r="E10" s="6" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="G10" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="H10">
         <v>1</v>
@@ -5888,13 +5969,13 @@
     </row>
     <row r="11" customFormat="1" spans="5:8">
       <c r="E11" s="6" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="G11" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="H11">
         <v>1</v>
@@ -5902,13 +5983,13 @@
     </row>
     <row r="12" customFormat="1" spans="5:8">
       <c r="E12" s="6" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="G12" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="H12">
         <v>1</v>
@@ -5916,13 +5997,13 @@
     </row>
     <row r="13" customFormat="1" spans="5:8">
       <c r="E13" s="6" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="G13" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="H13">
         <v>1</v>
@@ -5943,10 +6024,10 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:O52"/>
+  <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" topLeftCell="D19" workbookViewId="0">
+      <selection activeCell="E52" sqref="E52:E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.25"/>
@@ -6004,43 +6085,43 @@
         <v>50</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>53</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="H7" t="s">
         <v>56</v>
       </c>
       <c r="I7" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="J7" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="K7" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="L7" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="M7" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="N7" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="O7" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
     </row>
     <row r="8" customFormat="1" spans="1:14">
@@ -6049,20 +6130,20 @@
       <c r="C8" s="6"/>
       <c r="D8" s="1"/>
       <c r="E8" s="2" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="G8" s="6" t="str">
         <f>流水线模板任务分组!E11</f>
         <v>devops_ci_template_job_group-4</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="I8" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="J8">
         <v>0</v>
@@ -6077,25 +6158,25 @@
         <v>0</v>
       </c>
       <c r="N8" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
     </row>
     <row r="9" customFormat="1" spans="5:14">
       <c r="E9" s="6" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="G9" s="6" t="str">
         <f>流水线模板任务分组!E10</f>
         <v>devops_ci_template_job_group-3</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="I9" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="J9">
         <v>0</v>
@@ -6110,25 +6191,25 @@
         <v>0</v>
       </c>
       <c r="N9" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
     </row>
     <row r="10" customFormat="1" spans="5:14">
       <c r="E10" s="6" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="G10" s="6" t="str">
         <f>流水线模板任务分组!E9</f>
         <v>devops_ci_template_job_group-2</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="I10" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="J10">
         <v>0</v>
@@ -6143,25 +6224,25 @@
         <v>0</v>
       </c>
       <c r="N10" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
     </row>
     <row r="11" customFormat="1" spans="5:14">
       <c r="E11" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="G11" t="str">
         <f>流水线模板任务分组!E10</f>
         <v>devops_ci_template_job_group-3</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="I11" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="J11">
         <v>0</v>
@@ -6176,25 +6257,25 @@
         <v>0</v>
       </c>
       <c r="N11" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
     </row>
     <row r="12" spans="5:14">
       <c r="E12" s="8" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="F12" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="G12" t="str">
         <f>流水线模板任务分组!E9</f>
         <v>devops_ci_template_job_group-2</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="I12" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="J12">
         <v>0</v>
@@ -6209,25 +6290,25 @@
         <v>0</v>
       </c>
       <c r="N12" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
     </row>
     <row r="13" spans="5:14">
       <c r="E13" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="F13" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="G13" t="str">
         <f>流水线模板任务分组!E10</f>
         <v>devops_ci_template_job_group-3</v>
       </c>
       <c r="H13" s="9" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="I13" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="J13">
         <v>0</v>
@@ -6242,25 +6323,25 @@
         <v>0</v>
       </c>
       <c r="N13" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
     </row>
     <row r="14" spans="5:14">
       <c r="E14" s="6" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="F14" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="G14" t="str">
         <f>流水线模板任务分组!E9</f>
         <v>devops_ci_template_job_group-2</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="I14" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="J14">
         <v>0</v>
@@ -6275,25 +6356,25 @@
         <v>0</v>
       </c>
       <c r="N14" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
     </row>
     <row r="15" ht="20" customHeight="1" spans="5:14">
       <c r="E15" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="F15" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="G15" t="str">
         <f>流水线模板任务分组!E11</f>
         <v>devops_ci_template_job_group-4</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="I15" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="J15">
         <v>0</v>
@@ -6308,25 +6389,25 @@
         <v>0</v>
       </c>
       <c r="N15" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
     </row>
     <row r="16" spans="5:14">
       <c r="E16" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="F16" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="G16" t="str">
         <f>流水线模板任务分组!E10</f>
         <v>devops_ci_template_job_group-3</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="I16" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="J16">
         <v>0</v>
@@ -6341,25 +6422,25 @@
         <v>0</v>
       </c>
       <c r="N16" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
     </row>
     <row r="17" spans="5:14">
       <c r="E17" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="F17" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="G17" t="str">
         <f>流水线模板任务分组!E10</f>
         <v>devops_ci_template_job_group-3</v>
       </c>
       <c r="H17" s="9" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="I17" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="J17">
         <v>0</v>
@@ -6374,25 +6455,25 @@
         <v>0</v>
       </c>
       <c r="N17" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
     </row>
     <row r="18" spans="5:14">
       <c r="E18" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="F18" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="G18" t="str">
         <f>流水线模板任务分组!E10</f>
         <v>devops_ci_template_job_group-3</v>
       </c>
       <c r="H18" s="9" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="I18" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="J18">
         <v>0</v>
@@ -6407,22 +6488,22 @@
         <v>0</v>
       </c>
       <c r="N18" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
     </row>
     <row r="19" ht="362.25" spans="5:15">
       <c r="E19" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="F19" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="G19" t="str">
         <f>流水线模板任务分组!E8</f>
         <v>devops_ci_template_job_group-1</v>
       </c>
       <c r="I19" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="J19">
         <v>0</v>
@@ -6437,28 +6518,28 @@
         <v>0</v>
       </c>
       <c r="N19" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="O19" s="9" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
     </row>
     <row r="20" spans="5:15">
       <c r="E20" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="F20" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="G20" t="str">
         <f>流水线模板任务分组!E12</f>
         <v>devops_ci_template_job_group-5</v>
       </c>
       <c r="H20" s="9" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="I20" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="J20">
         <v>0</v>
@@ -6473,26 +6554,26 @@
         <v>0</v>
       </c>
       <c r="N20" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="O20" s="9"/>
     </row>
     <row r="21" spans="5:15">
       <c r="E21" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="F21" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="G21" t="str">
         <f>流水线模板任务分组!E12</f>
         <v>devops_ci_template_job_group-5</v>
       </c>
       <c r="H21" s="9" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="I21" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="J21">
         <v>0</v>
@@ -6507,26 +6588,26 @@
         <v>0</v>
       </c>
       <c r="N21" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="O21" s="9"/>
     </row>
     <row r="22" spans="5:15">
       <c r="E22" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="F22" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="G22" t="str">
         <f>流水线模板任务分组!E12</f>
         <v>devops_ci_template_job_group-5</v>
       </c>
       <c r="H22" s="9" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="I22" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="J22">
         <v>0</v>
@@ -6541,26 +6622,26 @@
         <v>0</v>
       </c>
       <c r="N22" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="O22" s="9"/>
     </row>
     <row r="23" spans="5:14">
       <c r="E23" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="F23" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="G23" t="str">
         <f>流水线模板任务分组!E13</f>
         <v>devops_ci_template_job_group-6</v>
       </c>
       <c r="H23" s="9" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="I23" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="J23">
         <v>0</v>
@@ -6575,25 +6656,25 @@
         <v>0</v>
       </c>
       <c r="N23" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
     </row>
     <row r="24" spans="5:14">
       <c r="E24" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="F24" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="G24" t="str">
         <f>流水线模板任务分组!E13</f>
         <v>devops_ci_template_job_group-6</v>
       </c>
       <c r="H24" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="I24" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="J24">
         <v>0</v>
@@ -6608,25 +6689,25 @@
         <v>0</v>
       </c>
       <c r="N24" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
     </row>
     <row r="25" spans="5:14">
       <c r="E25" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="F25" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="G25" t="str">
         <f>流水线模板任务分组!E13</f>
         <v>devops_ci_template_job_group-6</v>
       </c>
       <c r="H25" s="9" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="I25" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="J25">
         <v>0</v>
@@ -6641,25 +6722,25 @@
         <v>0</v>
       </c>
       <c r="N25" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
     </row>
     <row r="26" spans="5:14">
       <c r="E26" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="F26" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="G26" t="str">
         <f>流水线模板任务分组!E12</f>
         <v>devops_ci_template_job_group-5</v>
       </c>
       <c r="H26" s="9" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="I26" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="J26">
         <v>0</v>
@@ -6674,29 +6755,62 @@
         <v>0</v>
       </c>
       <c r="N26" t="s">
-        <v>162</v>
+        <v>167</v>
+      </c>
+    </row>
+    <row r="27" spans="5:14">
+      <c r="E27" t="s">
+        <v>213</v>
+      </c>
+      <c r="F27" t="s">
+        <v>214</v>
+      </c>
+      <c r="G27" t="str">
+        <f>流水线模板任务分组!E10</f>
+        <v>devops_ci_template_job_group-3</v>
+      </c>
+      <c r="H27" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="I27" t="s">
+        <v>90</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <v>1</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <v>0</v>
+      </c>
+      <c r="N27" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="29" spans="3:7">
       <c r="C29" t="s">
-        <v>208</v>
+        <v>215</v>
       </c>
       <c r="D29" t="s">
-        <v>209</v>
+        <v>216</v>
       </c>
       <c r="E29" t="s">
         <v>53</v>
       </c>
       <c r="F29" t="s">
-        <v>210</v>
+        <v>217</v>
       </c>
       <c r="G29" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
     </row>
     <row r="30" spans="5:7">
       <c r="E30" t="s">
-        <v>212</v>
+        <v>219</v>
       </c>
       <c r="F30" t="str">
         <f>流水线阶段模板!E8</f>
@@ -6709,7 +6823,7 @@
     </row>
     <row r="31" spans="5:7">
       <c r="E31" t="s">
-        <v>213</v>
+        <v>220</v>
       </c>
       <c r="F31" t="str">
         <f>流水线阶段模板!E8</f>
@@ -6722,7 +6836,7 @@
     </row>
     <row r="32" spans="5:7">
       <c r="E32" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="F32" t="str">
         <f>流水线阶段模板!E9</f>
@@ -6735,7 +6849,7 @@
     </row>
     <row r="33" spans="5:7">
       <c r="E33" t="s">
-        <v>215</v>
+        <v>222</v>
       </c>
       <c r="F33" t="str">
         <f>流水线阶段模板!E10</f>
@@ -6748,7 +6862,7 @@
     </row>
     <row r="34" spans="5:7">
       <c r="E34" t="s">
-        <v>216</v>
+        <v>223</v>
       </c>
       <c r="F34" t="str">
         <f>流水线阶段模板!E10</f>
@@ -6761,7 +6875,7 @@
     </row>
     <row r="35" spans="5:7">
       <c r="E35" t="s">
-        <v>217</v>
+        <v>224</v>
       </c>
       <c r="F35" t="str">
         <f>流水线阶段模板!E11</f>
@@ -6774,7 +6888,7 @@
     </row>
     <row r="36" spans="5:7">
       <c r="E36" t="s">
-        <v>218</v>
+        <v>225</v>
       </c>
       <c r="F36" t="str">
         <f>流水线阶段模板!E12</f>
@@ -6787,7 +6901,7 @@
     </row>
     <row r="37" spans="5:7">
       <c r="E37" t="s">
-        <v>219</v>
+        <v>226</v>
       </c>
       <c r="F37" t="str">
         <f>流水线阶段模板!E12</f>
@@ -6800,7 +6914,7 @@
     </row>
     <row r="38" spans="5:7">
       <c r="E38" t="s">
-        <v>220</v>
+        <v>227</v>
       </c>
       <c r="F38" t="str">
         <f>流水线阶段模板!E13</f>
@@ -6813,7 +6927,7 @@
     </row>
     <row r="39" spans="5:7">
       <c r="E39" s="8" t="s">
-        <v>221</v>
+        <v>228</v>
       </c>
       <c r="F39" t="str">
         <f>流水线阶段模板!E14</f>
@@ -6826,7 +6940,7 @@
     </row>
     <row r="40" spans="5:7">
       <c r="E40" s="8" t="s">
-        <v>222</v>
+        <v>229</v>
       </c>
       <c r="F40" t="str">
         <f>流水线阶段模板!E14</f>
@@ -6839,7 +6953,7 @@
     </row>
     <row r="41" spans="5:7">
       <c r="E41" s="8" t="s">
-        <v>223</v>
+        <v>230</v>
       </c>
       <c r="F41" t="str">
         <f>流水线阶段模板!E15</f>
@@ -6852,7 +6966,7 @@
     </row>
     <row r="42" spans="5:7">
       <c r="E42" s="6" t="s">
-        <v>224</v>
+        <v>231</v>
       </c>
       <c r="F42" t="str">
         <f>流水线阶段模板!E16</f>
@@ -6865,7 +6979,7 @@
     </row>
     <row r="43" spans="5:7">
       <c r="E43" t="s">
-        <v>225</v>
+        <v>232</v>
       </c>
       <c r="F43" t="str">
         <f>流水线阶段模板!E16</f>
@@ -6878,7 +6992,7 @@
     </row>
     <row r="44" spans="5:7">
       <c r="E44" t="s">
-        <v>226</v>
+        <v>233</v>
       </c>
       <c r="F44" t="str">
         <f>流水线阶段模板!E17</f>
@@ -6891,7 +7005,7 @@
     </row>
     <row r="45" spans="5:7">
       <c r="E45" t="s">
-        <v>227</v>
+        <v>234</v>
       </c>
       <c r="F45" t="str">
         <f>流水线阶段模板!E18</f>
@@ -6904,7 +7018,7 @@
     </row>
     <row r="46" spans="5:7">
       <c r="E46" t="s">
-        <v>228</v>
+        <v>235</v>
       </c>
       <c r="F46" t="str">
         <f>流水线阶段模板!E18</f>
@@ -6917,7 +7031,7 @@
     </row>
     <row r="47" spans="5:7">
       <c r="E47" s="6" t="s">
-        <v>229</v>
+        <v>236</v>
       </c>
       <c r="F47" t="str">
         <f>流水线阶段模板!E19</f>
@@ -6930,7 +7044,7 @@
     </row>
     <row r="48" spans="5:7">
       <c r="E48" t="s">
-        <v>230</v>
+        <v>237</v>
       </c>
       <c r="F48" t="str">
         <f>流水线阶段模板!E20</f>
@@ -6943,7 +7057,7 @@
     </row>
     <row r="49" spans="5:7">
       <c r="E49" t="s">
-        <v>231</v>
+        <v>238</v>
       </c>
       <c r="F49" t="str">
         <f>流水线阶段模板!E21</f>
@@ -6956,7 +7070,7 @@
     </row>
     <row r="50" spans="5:7">
       <c r="E50" t="s">
-        <v>232</v>
+        <v>239</v>
       </c>
       <c r="F50" t="str">
         <f>流水线阶段模板!E22</f>
@@ -6969,7 +7083,7 @@
     </row>
     <row r="51" spans="5:7">
       <c r="E51" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="F51" t="str">
         <f>流水线阶段模板!E23</f>
@@ -6982,7 +7096,7 @@
     </row>
     <row r="52" spans="5:7">
       <c r="E52" t="s">
-        <v>234</v>
+        <v>241</v>
       </c>
       <c r="F52" t="str">
         <f>流水线阶段模板!E24</f>
@@ -6991,6 +7105,19 @@
       <c r="G52" t="str">
         <f>E18</f>
         <v>devops_ci_template_job-20</v>
+      </c>
+    </row>
+    <row r="53" spans="5:7">
+      <c r="E53" t="s">
+        <v>242</v>
+      </c>
+      <c r="F53" t="str">
+        <f>流水线阶段模板!E25</f>
+        <v>devops_ci_template_stage-18</v>
+      </c>
+      <c r="G53" t="str">
+        <f>E27</f>
+        <v>devops_ci_template_job-29</v>
       </c>
     </row>
   </sheetData>
@@ -7052,19 +7179,19 @@
         <v>50</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>235</v>
+        <v>243</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>53</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" customFormat="1" spans="1:7">
@@ -7073,7 +7200,7 @@
       <c r="C8" s="6"/>
       <c r="D8" s="1"/>
       <c r="E8" s="2" t="s">
-        <v>236</v>
+        <v>244</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>58</v>
@@ -7084,10 +7211,10 @@
     </row>
     <row r="9" customFormat="1" spans="5:7">
       <c r="E9" s="6" t="s">
-        <v>237</v>
+        <v>245</v>
       </c>
       <c r="F9" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="G9">
         <v>1</v>
@@ -7095,10 +7222,10 @@
     </row>
     <row r="10" customFormat="1" spans="5:7">
       <c r="E10" s="6" t="s">
-        <v>238</v>
+        <v>246</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="G10">
         <v>1</v>
@@ -7106,10 +7233,10 @@
     </row>
     <row r="11" customFormat="1" spans="5:7">
       <c r="E11" s="6" t="s">
-        <v>239</v>
+        <v>247</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="G11">
         <v>1</v>
@@ -7117,10 +7244,10 @@
     </row>
     <row r="12" customFormat="1" spans="5:7">
       <c r="E12" s="6" t="s">
-        <v>240</v>
+        <v>248</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="G12">
         <v>1</v>
@@ -7141,10 +7268,10 @@
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:L62"/>
+  <dimension ref="A1:L64"/>
   <sheetViews>
-    <sheetView zoomScale="81" zoomScaleNormal="81" topLeftCell="D20" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+    <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="81" topLeftCell="D35" workbookViewId="0">
+      <selection activeCell="H64" sqref="H64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.25"/>
@@ -7199,34 +7326,34 @@
         <v>50</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>242</v>
+        <v>250</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>53</v>
       </c>
       <c r="F7" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="H7" t="s">
         <v>83</v>
       </c>
-      <c r="G7" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="H7" t="s">
-        <v>81</v>
-      </c>
       <c r="I7" t="s">
-        <v>243</v>
+        <v>251</v>
       </c>
       <c r="J7" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="K7" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="L7" s="6" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" customFormat="1" spans="1:12">
@@ -7235,23 +7362,23 @@
       <c r="C8" s="6"/>
       <c r="D8" s="1"/>
       <c r="E8" s="2" t="s">
-        <v>244</v>
+        <v>252</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>245</v>
+        <v>253</v>
       </c>
       <c r="G8" s="6">
         <v>0</v>
       </c>
       <c r="H8" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I8" t="str">
         <f>流水线步骤分类!E11</f>
         <v>devops_ci_template_step_category-4</v>
       </c>
       <c r="J8" t="s">
-        <v>246</v>
+        <v>254</v>
       </c>
       <c r="L8">
         <v>1</v>
@@ -7263,26 +7390,26 @@
       <c r="C9" s="6"/>
       <c r="D9" s="1"/>
       <c r="E9" s="2" t="s">
-        <v>247</v>
+        <v>255</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="G9" s="6">
         <v>0</v>
       </c>
       <c r="H9" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I9" t="str">
         <f>流水线步骤分类!E10</f>
         <v>devops_ci_template_step_category-3</v>
       </c>
       <c r="J9" t="s">
-        <v>248</v>
+        <v>256</v>
       </c>
       <c r="K9" s="9" t="s">
-        <v>249</v>
+        <v>257</v>
       </c>
       <c r="L9">
         <v>1</v>
@@ -7290,26 +7417,26 @@
     </row>
     <row r="10" customFormat="1" ht="327.75" spans="5:12">
       <c r="E10" s="6" t="s">
-        <v>250</v>
+        <v>258</v>
       </c>
       <c r="F10" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="G10" s="6">
         <v>0</v>
       </c>
       <c r="H10" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I10" t="str">
         <f>流水线步骤分类!E9</f>
         <v>devops_ci_template_step_category-2</v>
       </c>
       <c r="J10" t="s">
-        <v>251</v>
+        <v>259</v>
       </c>
       <c r="K10" s="9" t="s">
-        <v>252</v>
+        <v>260</v>
       </c>
       <c r="L10">
         <v>1</v>
@@ -7317,23 +7444,23 @@
     </row>
     <row r="11" customFormat="1" spans="5:12">
       <c r="E11" s="6" t="s">
-        <v>253</v>
+        <v>261</v>
       </c>
       <c r="F11" t="s">
-        <v>254</v>
+        <v>262</v>
       </c>
       <c r="G11" s="6">
         <v>0</v>
       </c>
       <c r="H11" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I11" t="str">
         <f>流水线步骤分类!E9</f>
         <v>devops_ci_template_step_category-2</v>
       </c>
       <c r="J11" t="s">
-        <v>255</v>
+        <v>263</v>
       </c>
       <c r="L11">
         <v>1</v>
@@ -7341,23 +7468,23 @@
     </row>
     <row r="12" customFormat="1" spans="5:12">
       <c r="E12" s="6" t="s">
-        <v>256</v>
+        <v>264</v>
       </c>
       <c r="F12" t="s">
-        <v>257</v>
+        <v>265</v>
       </c>
       <c r="G12" s="6">
         <v>0</v>
       </c>
       <c r="H12" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I12" t="str">
         <f>流水线步骤分类!E12</f>
         <v>devops_ci_template_step_category-5</v>
       </c>
       <c r="J12" t="s">
-        <v>258</v>
+        <v>266</v>
       </c>
       <c r="L12">
         <v>1</v>
@@ -7365,26 +7492,26 @@
     </row>
     <row r="13" customFormat="1" ht="409.5" spans="5:12">
       <c r="E13" s="6" t="s">
-        <v>259</v>
+        <v>267</v>
       </c>
       <c r="F13" t="s">
-        <v>260</v>
+        <v>268</v>
       </c>
       <c r="G13" s="6">
         <v>0</v>
       </c>
       <c r="H13" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I13" t="str">
         <f>流水线步骤分类!E12</f>
         <v>devops_ci_template_step_category-5</v>
       </c>
       <c r="J13" t="s">
-        <v>261</v>
+        <v>269</v>
       </c>
       <c r="K13" s="9" t="s">
-        <v>262</v>
+        <v>270</v>
       </c>
       <c r="L13">
         <v>1</v>
@@ -7392,26 +7519,26 @@
     </row>
     <row r="14" customFormat="1" ht="86.25" spans="5:12">
       <c r="E14" s="6" t="s">
-        <v>263</v>
+        <v>271</v>
       </c>
       <c r="F14" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="G14" s="6">
         <v>0</v>
       </c>
       <c r="H14" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I14" t="str">
         <f>流水线步骤分类!E10</f>
         <v>devops_ci_template_step_category-3</v>
       </c>
       <c r="J14" t="s">
-        <v>264</v>
+        <v>272</v>
       </c>
       <c r="K14" s="9" t="s">
-        <v>265</v>
+        <v>273</v>
       </c>
       <c r="L14">
         <v>1</v>
@@ -7419,26 +7546,26 @@
     </row>
     <row r="15" customFormat="1" spans="5:12">
       <c r="E15" s="8" t="s">
-        <v>266</v>
+        <v>274</v>
       </c>
       <c r="F15" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="G15" s="6">
         <v>0</v>
       </c>
       <c r="H15" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I15" t="str">
         <f>流水线步骤分类!E9</f>
         <v>devops_ci_template_step_category-2</v>
       </c>
       <c r="J15" t="s">
-        <v>267</v>
+        <v>275</v>
       </c>
       <c r="K15" t="s">
-        <v>268</v>
+        <v>276</v>
       </c>
       <c r="L15">
         <v>1</v>
@@ -7446,23 +7573,23 @@
     </row>
     <row r="16" customFormat="1" spans="5:12">
       <c r="E16" s="6" t="s">
-        <v>269</v>
+        <v>277</v>
       </c>
       <c r="F16" t="s">
-        <v>254</v>
+        <v>262</v>
       </c>
       <c r="G16" s="6">
         <v>0</v>
       </c>
       <c r="H16" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I16" t="str">
         <f>流水线步骤分类!E9</f>
         <v>devops_ci_template_step_category-2</v>
       </c>
       <c r="J16" t="s">
-        <v>255</v>
+        <v>263</v>
       </c>
       <c r="L16">
         <v>1</v>
@@ -7470,26 +7597,26 @@
     </row>
     <row r="17" customFormat="1" ht="189.75" spans="5:12">
       <c r="E17" s="6" t="s">
-        <v>270</v>
+        <v>278</v>
       </c>
       <c r="F17" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="G17" s="6">
         <v>0</v>
       </c>
       <c r="H17" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I17" t="str">
         <f>流水线步骤分类!E10</f>
         <v>devops_ci_template_step_category-3</v>
       </c>
       <c r="J17" t="s">
-        <v>271</v>
+        <v>279</v>
       </c>
       <c r="K17" s="9" t="s">
-        <v>272</v>
+        <v>280</v>
       </c>
       <c r="L17">
         <v>1</v>
@@ -7497,23 +7624,23 @@
     </row>
     <row r="18" customFormat="1" spans="5:12">
       <c r="E18" s="8" t="s">
-        <v>273</v>
+        <v>281</v>
       </c>
       <c r="F18" t="s">
-        <v>274</v>
+        <v>282</v>
       </c>
       <c r="G18" s="6">
         <v>0</v>
       </c>
       <c r="H18" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I18" t="str">
         <f>流水线步骤分类!E9</f>
         <v>devops_ci_template_step_category-2</v>
       </c>
       <c r="J18" t="s">
-        <v>275</v>
+        <v>283</v>
       </c>
       <c r="L18">
         <v>1</v>
@@ -7521,26 +7648,26 @@
     </row>
     <row r="19" customFormat="1" ht="207" spans="5:12">
       <c r="E19" s="6" t="s">
-        <v>276</v>
+        <v>284</v>
       </c>
       <c r="F19" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="G19" s="6">
         <v>0</v>
       </c>
       <c r="H19" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I19" t="str">
         <f>流水线步骤分类!E9</f>
         <v>devops_ci_template_step_category-2</v>
       </c>
       <c r="J19" t="s">
-        <v>277</v>
+        <v>285</v>
       </c>
       <c r="K19" s="9" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="L19">
         <v>1</v>
@@ -7548,26 +7675,26 @@
     </row>
     <row r="20" customFormat="1" ht="241.5" spans="5:12">
       <c r="E20" s="6" t="s">
-        <v>279</v>
+        <v>287</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>280</v>
+        <v>288</v>
       </c>
       <c r="G20" s="6">
         <v>0</v>
       </c>
       <c r="H20" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I20" t="str">
         <f>流水线步骤分类!E9</f>
         <v>devops_ci_template_step_category-2</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>281</v>
+        <v>289</v>
       </c>
       <c r="K20" s="9" t="s">
-        <v>282</v>
+        <v>290</v>
       </c>
       <c r="L20">
         <v>1</v>
@@ -7575,23 +7702,23 @@
     </row>
     <row r="21" customFormat="1" ht="47" customHeight="1" spans="5:12">
       <c r="E21" s="6" t="s">
-        <v>283</v>
+        <v>291</v>
       </c>
       <c r="F21" t="s">
-        <v>284</v>
+        <v>292</v>
       </c>
       <c r="G21" s="6">
         <v>0</v>
       </c>
       <c r="H21" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I21" t="str">
         <f>流水线步骤分类!E11</f>
         <v>devops_ci_template_step_category-4</v>
       </c>
       <c r="J21" t="s">
-        <v>246</v>
+        <v>254</v>
       </c>
       <c r="L21">
         <v>1</v>
@@ -7599,26 +7726,26 @@
     </row>
     <row r="22" customFormat="1" spans="5:12">
       <c r="E22" s="6" t="s">
-        <v>285</v>
+        <v>293</v>
       </c>
       <c r="F22" t="s">
-        <v>286</v>
+        <v>294</v>
       </c>
       <c r="G22" s="6">
         <v>0</v>
       </c>
       <c r="H22" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I22" t="str">
         <f>流水线步骤分类!E12</f>
         <v>devops_ci_template_step_category-5</v>
       </c>
       <c r="J22" t="s">
-        <v>287</v>
+        <v>295</v>
       </c>
       <c r="K22" t="s">
-        <v>288</v>
+        <v>296</v>
       </c>
       <c r="L22">
         <v>1</v>
@@ -7626,26 +7753,26 @@
     </row>
     <row r="23" customFormat="1" ht="48" customHeight="1" spans="5:12">
       <c r="E23" s="6" t="s">
-        <v>289</v>
+        <v>297</v>
       </c>
       <c r="F23" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="G23" s="6">
         <v>0</v>
       </c>
       <c r="H23" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I23" t="str">
         <f>流水线步骤分类!E10</f>
         <v>devops_ci_template_step_category-3</v>
       </c>
       <c r="J23" t="s">
-        <v>290</v>
+        <v>298</v>
       </c>
       <c r="K23" s="9" t="s">
-        <v>291</v>
+        <v>299</v>
       </c>
       <c r="L23">
         <v>1</v>
@@ -7653,26 +7780,26 @@
     </row>
     <row r="24" spans="5:12">
       <c r="E24" t="s">
-        <v>292</v>
+        <v>300</v>
       </c>
       <c r="F24" t="s">
-        <v>293</v>
+        <v>301</v>
       </c>
       <c r="G24">
         <v>0</v>
       </c>
       <c r="H24" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I24" t="str">
         <f>流水线步骤分类!E8</f>
         <v>devops_ci_template_step_category-1</v>
       </c>
       <c r="J24" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="K24" t="s">
-        <v>294</v>
+        <v>302</v>
       </c>
       <c r="L24">
         <v>1</v>
@@ -7680,24 +7807,24 @@
     </row>
     <row r="29" spans="4:8">
       <c r="D29" t="s">
-        <v>295</v>
+        <v>303</v>
       </c>
       <c r="E29" t="s">
         <v>53</v>
       </c>
       <c r="F29" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="G29" t="s">
-        <v>296</v>
+        <v>304</v>
       </c>
       <c r="H29" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
     </row>
     <row r="30" spans="5:8">
       <c r="E30" t="s">
-        <v>297</v>
+        <v>305</v>
       </c>
       <c r="F30" t="str">
         <f>流水线任务模板!E8</f>
@@ -7713,7 +7840,7 @@
     </row>
     <row r="31" spans="5:8">
       <c r="E31" t="s">
-        <v>298</v>
+        <v>306</v>
       </c>
       <c r="F31" t="str">
         <f>流水线任务模板!E9</f>
@@ -7729,7 +7856,7 @@
     </row>
     <row r="32" spans="5:8">
       <c r="E32" t="s">
-        <v>299</v>
+        <v>307</v>
       </c>
       <c r="F32" t="str">
         <f>流水线任务模板!E9</f>
@@ -7745,7 +7872,7 @@
     </row>
     <row r="33" spans="5:8">
       <c r="E33" t="s">
-        <v>300</v>
+        <v>308</v>
       </c>
       <c r="F33" t="str">
         <f>流水线任务模板!E9</f>
@@ -7761,7 +7888,7 @@
     </row>
     <row r="34" spans="5:8">
       <c r="E34" t="s">
-        <v>301</v>
+        <v>309</v>
       </c>
       <c r="F34" t="str">
         <f>流水线任务模板!E10</f>
@@ -7777,7 +7904,7 @@
     </row>
     <row r="35" spans="5:8">
       <c r="E35" t="s">
-        <v>302</v>
+        <v>310</v>
       </c>
       <c r="F35" t="str">
         <f>流水线任务模板!E10</f>
@@ -7793,7 +7920,7 @@
     </row>
     <row r="36" spans="5:8">
       <c r="E36" t="s">
-        <v>303</v>
+        <v>311</v>
       </c>
       <c r="F36" t="str">
         <f>流水线任务模板!E11</f>
@@ -7809,7 +7936,7 @@
     </row>
     <row r="37" spans="5:8">
       <c r="E37" t="s">
-        <v>304</v>
+        <v>312</v>
       </c>
       <c r="F37" t="str">
         <f>流水线任务模板!E11</f>
@@ -7825,7 +7952,7 @@
     </row>
     <row r="38" spans="5:8">
       <c r="E38" s="8" t="s">
-        <v>305</v>
+        <v>313</v>
       </c>
       <c r="F38" t="str">
         <f>流水线任务模板!E12</f>
@@ -7841,7 +7968,7 @@
     </row>
     <row r="39" spans="5:8">
       <c r="E39" t="s">
-        <v>306</v>
+        <v>314</v>
       </c>
       <c r="F39" t="str">
         <f>流水线任务模板!E13</f>
@@ -7857,7 +7984,7 @@
     </row>
     <row r="40" spans="5:8">
       <c r="E40" t="s">
-        <v>307</v>
+        <v>315</v>
       </c>
       <c r="F40" t="str">
         <f>流水线任务模板!E13</f>
@@ -7873,7 +8000,7 @@
     </row>
     <row r="41" spans="5:8">
       <c r="E41" t="s">
-        <v>308</v>
+        <v>316</v>
       </c>
       <c r="F41" t="str">
         <f>流水线任务模板!E13</f>
@@ -7889,7 +8016,7 @@
     </row>
     <row r="42" spans="5:8">
       <c r="E42" s="6" t="s">
-        <v>309</v>
+        <v>317</v>
       </c>
       <c r="F42" t="str">
         <f>流水线任务模板!E14</f>
@@ -7905,7 +8032,7 @@
     </row>
     <row r="43" spans="5:8">
       <c r="E43" t="s">
-        <v>310</v>
+        <v>318</v>
       </c>
       <c r="F43" t="str">
         <f>流水线任务模板!E15</f>
@@ -7921,7 +8048,7 @@
     </row>
     <row r="44" spans="5:8">
       <c r="E44" t="s">
-        <v>311</v>
+        <v>319</v>
       </c>
       <c r="F44" t="str">
         <f>流水线任务模板!E16</f>
@@ -7937,7 +8064,7 @@
     </row>
     <row r="45" spans="5:8">
       <c r="E45" t="s">
-        <v>312</v>
+        <v>320</v>
       </c>
       <c r="F45" t="str">
         <f>流水线任务模板!E16</f>
@@ -7953,7 +8080,7 @@
     </row>
     <row r="46" spans="5:8">
       <c r="E46" t="s">
-        <v>313</v>
+        <v>321</v>
       </c>
       <c r="F46" t="str">
         <f>流水线任务模板!E17</f>
@@ -7969,7 +8096,7 @@
     </row>
     <row r="47" spans="5:8">
       <c r="E47" t="s">
-        <v>314</v>
+        <v>322</v>
       </c>
       <c r="F47" t="str">
         <f>流水线任务模板!E17</f>
@@ -7985,7 +8112,7 @@
     </row>
     <row r="48" spans="5:8">
       <c r="E48" t="s">
-        <v>315</v>
+        <v>323</v>
       </c>
       <c r="F48" t="str">
         <f>流水线任务模板!E18</f>
@@ -8001,7 +8128,7 @@
     </row>
     <row r="49" spans="5:8">
       <c r="E49" t="s">
-        <v>316</v>
+        <v>324</v>
       </c>
       <c r="F49" t="str">
         <f>流水线任务模板!E18</f>
@@ -8017,7 +8144,7 @@
     </row>
     <row r="50" spans="5:8">
       <c r="E50" t="s">
-        <v>317</v>
+        <v>325</v>
       </c>
       <c r="F50" t="str">
         <f>流水线任务模板!E20</f>
@@ -8033,7 +8160,7 @@
     </row>
     <row r="51" spans="5:8">
       <c r="E51" t="s">
-        <v>318</v>
+        <v>326</v>
       </c>
       <c r="F51" t="str">
         <f>流水线任务模板!E21</f>
@@ -8049,7 +8176,7 @@
     </row>
     <row r="52" spans="5:8">
       <c r="E52" t="s">
-        <v>319</v>
+        <v>327</v>
       </c>
       <c r="F52" t="str">
         <f>流水线任务模板!E22</f>
@@ -8065,7 +8192,7 @@
     </row>
     <row r="53" spans="5:8">
       <c r="E53" t="s">
-        <v>320</v>
+        <v>328</v>
       </c>
       <c r="F53" t="str">
         <f>流水线任务模板!E14</f>
@@ -8081,7 +8208,7 @@
     </row>
     <row r="54" spans="5:8">
       <c r="E54" t="s">
-        <v>321</v>
+        <v>329</v>
       </c>
       <c r="F54" t="str">
         <f>流水线任务模板!E23</f>
@@ -8097,7 +8224,7 @@
     </row>
     <row r="55" spans="5:8">
       <c r="E55" t="s">
-        <v>322</v>
+        <v>330</v>
       </c>
       <c r="F55" t="str">
         <f>流水线任务模板!E23</f>
@@ -8113,7 +8240,7 @@
     </row>
     <row r="56" spans="5:8">
       <c r="E56" t="s">
-        <v>323</v>
+        <v>331</v>
       </c>
       <c r="F56" t="str">
         <f>流水线任务模板!E23</f>
@@ -8129,7 +8256,7 @@
     </row>
     <row r="57" spans="5:8">
       <c r="E57" t="s">
-        <v>324</v>
+        <v>332</v>
       </c>
       <c r="F57" t="str">
         <f>流水线任务模板!E24</f>
@@ -8145,7 +8272,7 @@
     </row>
     <row r="58" spans="5:8">
       <c r="E58" t="s">
-        <v>325</v>
+        <v>333</v>
       </c>
       <c r="F58" t="str">
         <f>流水线任务模板!E24</f>
@@ -8161,7 +8288,7 @@
     </row>
     <row r="59" spans="5:8">
       <c r="E59" t="s">
-        <v>326</v>
+        <v>334</v>
       </c>
       <c r="F59" t="str">
         <f>流水线任务模板!E25</f>
@@ -8177,7 +8304,7 @@
     </row>
     <row r="60" spans="5:8">
       <c r="E60" t="s">
-        <v>327</v>
+        <v>335</v>
       </c>
       <c r="F60" t="str">
         <f>流水线任务模板!E25</f>
@@ -8193,7 +8320,7 @@
     </row>
     <row r="61" spans="5:8">
       <c r="E61" t="s">
-        <v>328</v>
+        <v>336</v>
       </c>
       <c r="F61" t="str">
         <f>流水线任务模板!E25</f>
@@ -8209,7 +8336,7 @@
     </row>
     <row r="62" spans="5:8">
       <c r="E62" t="s">
-        <v>329</v>
+        <v>337</v>
       </c>
       <c r="F62" t="str">
         <f>流水线任务模板!E26</f>
@@ -8221,6 +8348,38 @@
       </c>
       <c r="H62">
         <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="5:8">
+      <c r="E63" t="s">
+        <v>338</v>
+      </c>
+      <c r="F63" t="str">
+        <f>流水线任务模板!E27</f>
+        <v>devops_ci_template_job-29</v>
+      </c>
+      <c r="G63" t="str">
+        <f>E16</f>
+        <v>devops_ci_template_step-9</v>
+      </c>
+      <c r="H63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="5:8">
+      <c r="E64" t="s">
+        <v>339</v>
+      </c>
+      <c r="F64" t="str">
+        <f>流水线任务模板!E27</f>
+        <v>devops_ci_template_job-29</v>
+      </c>
+      <c r="G64" t="str">
+        <f>E12</f>
+        <v>devops_ci_template_step-5</v>
+      </c>
+      <c r="H64">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>